<commit_message>
Add files for task4 and change task2 table
</commit_message>
<xml_diff>
--- a/Checklists/Task2/solution_t2.xlsx
+++ b/Checklists/Task2/solution_t2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\QA_Portfolio\Checklists\Task2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AA33D3-27F0-4CEF-B871-18E6124C427E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C2007B-415A-46A8-8AC4-0CFF96609E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,6 +98,8 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>https://retromagaz.com/games-ps5</t>
@@ -225,7 +227,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,12 +239,25 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -299,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -311,6 +326,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,13 +627,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>